<commit_message>
Changed labels to reflect program output
</commit_message>
<xml_diff>
--- a/latinsquare/latinsquarematrix.xlsx
+++ b/latinsquare/latinsquarematrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\IdeaProjects\sudoku project\src\latinsqaure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\IdeaProjects\sudoku project\src\latinsquare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64BF5EFB-217C-44B0-A078-D7E44125697F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3AFB30-AD79-4264-BBAF-2A18CBB70F21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{21DB58CE-3E54-4BBD-A338-BE5D7C90EF89}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Row</t>
   </si>
   <si>
-    <t>(col, row)</t>
-  </si>
-  <si>
     <t>1 : (1,1)</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>or</t>
+  </si>
+  <si>
+    <t>(row, col)</t>
   </si>
 </sst>
 </file>
@@ -88,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,7 +97,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,15 +170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -186,11 +186,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +515,7 @@
   <dimension ref="C2:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,321 +525,316 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
+        <v>2</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8">
+        <v>2</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8">
+        <v>1</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8">
+        <v>2</v>
+      </c>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="6">
+        <v>2</v>
+      </c>
+      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="11"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3">
-        <v>2</v>
-      </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>2</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
-        <v>2</v>
-      </c>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
-        <v>2</v>
-      </c>
-      <c r="L6" s="8">
-        <v>1</v>
-      </c>
-      <c r="M6" s="8">
-        <v>2</v>
-      </c>
-      <c r="N6" s="8">
-        <v>1</v>
-      </c>
-      <c r="O6" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
         <v>2</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="5">
-        <v>2</v>
-      </c>
-      <c r="K18" s="5">
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="5">
-        <v>2</v>
-      </c>
-      <c r="F19" s="5">
+      <c r="E19" s="3">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
         <v>1</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="5">
-        <v>1</v>
-      </c>
-      <c r="K19" s="5">
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="D2:O2"/>
     <mergeCell ref="E16:K16"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="D4:E4"/>
@@ -842,6 +844,11 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="H5:K5"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="D2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to show rows for each solution
</commit_message>
<xml_diff>
--- a/latinsquare/latinsquarematrix.xlsx
+++ b/latinsquare/latinsquarematrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\IdeaProjects\sudoku project\src\latinsquare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3AFB30-AD79-4264-BBAF-2A18CBB70F21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3212BE79-A29C-4843-B8A2-8C671FD5E693}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{21DB58CE-3E54-4BBD-A338-BE5D7C90EF89}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Candidate</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Possible Solutions</t>
-  </si>
-  <si>
-    <t>or</t>
   </si>
   <si>
     <t>(row, col)</t>
@@ -170,15 +167,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -190,14 +181,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,330 +511,525 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C4986-8F4F-4072-9000-5A8C4AA38561}">
-  <dimension ref="C2:O19"/>
+  <dimension ref="B2:AD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="15" width="4.42578125" customWidth="1"/>
+    <col min="19" max="30" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="9" t="s">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D3" s="8" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="V2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
-        <v>2</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8">
-        <v>2</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8">
-        <v>1</v>
-      </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8">
-        <v>2</v>
-      </c>
-      <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10">
+        <v>2</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10">
+        <v>2</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="W4" s="6">
+        <v>1</v>
+      </c>
+      <c r="X4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>2</v>
-      </c>
-      <c r="J6" s="6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="6">
-        <v>2</v>
-      </c>
-      <c r="L6" s="6">
-        <v>1</v>
-      </c>
-      <c r="M6" s="6">
-        <v>2</v>
-      </c>
-      <c r="N6" s="6">
-        <v>1</v>
-      </c>
-      <c r="O6" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="D5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="W5" s="6">
+        <v>2</v>
+      </c>
+      <c r="X5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="7"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="7"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="1"/>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="11"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="7"/>
+      <c r="Q10">
+        <v>6</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="1"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="W12" s="6">
+        <v>2</v>
+      </c>
+      <c r="X12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="1"/>
+      <c r="W13" s="6">
+        <v>1</v>
+      </c>
+      <c r="X13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="11"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="3">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="3">
-        <v>2</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3">
-        <v>2</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S15" s="7"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="1"/>
+    </row>
+    <row r="17" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+    </row>
+    <row r="18" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="Q18">
+        <v>7</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="7"/>
+    </row>
+    <row r="19" spans="5:30" x14ac:dyDescent="0.25">
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="D2:O2"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
@@ -844,11 +1038,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="H5:K5"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="D2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>